<commit_message>
Added Future Ticker Codes
</commit_message>
<xml_diff>
--- a/Futures/Futures.xlsx
+++ b/Futures/Futures.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Futures" sheetId="1" r:id="rId1"/>
+    <sheet name="Tickers" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>r</t>
   </si>
@@ -139,6 +140,57 @@
   <si>
     <t>https://www.cmegroup.com/education/files/sofr-futures-contract-specifications.pdf</t>
   </si>
+  <si>
+    <t>Product Code</t>
+  </si>
+  <si>
+    <t>Month Code</t>
+  </si>
+  <si>
+    <t>Year Code</t>
+  </si>
+  <si>
+    <t>ED</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Ticker</t>
+  </si>
+  <si>
+    <t>Eurodollar Futures DEC-2023</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Expiry</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>Z3</t>
+  </si>
+  <si>
+    <t>Eurodollar Futures MAR-2023</t>
+  </si>
+  <si>
+    <t>Eurodollar Futures JUN-2023</t>
+  </si>
+  <si>
+    <t>Eurodollar Futures SEP-2023</t>
+  </si>
 </sst>
 </file>
 
@@ -148,7 +200,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.00000"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,8 +230,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -192,8 +273,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -212,11 +311,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -244,6 +432,96 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -268,8 +546,8 @@
       <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2951129" cy="305405"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -373,7 +651,7 @@
                             <a:schemeClr val="tx1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
+                          <a:latin typeface="Cambria Math"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -391,7 +669,7 @@
                                 <a:schemeClr val="tx1"/>
                               </a:solidFill>
                               <a:effectLst/>
-                              <a:latin typeface="+mn-lt"/>
+                              <a:latin typeface="Cambria Math"/>
                               <a:ea typeface="+mn-ea"/>
                               <a:cs typeface="+mn-cs"/>
                             </a:rPr>
@@ -407,7 +685,7 @@
                                 <a:schemeClr val="tx1"/>
                               </a:solidFill>
                               <a:effectLst/>
-                              <a:latin typeface="+mn-lt"/>
+                              <a:latin typeface="Cambria Math"/>
                               <a:ea typeface="+mn-ea"/>
                               <a:cs typeface="+mn-cs"/>
                             </a:rPr>
@@ -426,7 +704,7 @@
                                     <a:schemeClr val="tx1"/>
                                   </a:solidFill>
                                   <a:effectLst/>
-                                  <a:latin typeface="+mn-lt"/>
+                                  <a:latin typeface="Cambria Math"/>
                                   <a:ea typeface="+mn-ea"/>
                                   <a:cs typeface="+mn-cs"/>
                                 </a:rPr>
@@ -439,7 +717,7 @@
                                     <a:schemeClr val="tx1"/>
                                   </a:solidFill>
                                   <a:effectLst/>
-                                  <a:latin typeface="+mn-lt"/>
+                                  <a:latin typeface="Cambria Math"/>
                                   <a:ea typeface="+mn-ea"/>
                                   <a:cs typeface="+mn-cs"/>
                                 </a:rPr>
@@ -453,7 +731,7 @@
                                         <a:schemeClr val="tx1"/>
                                       </a:solidFill>
                                       <a:effectLst/>
-                                      <a:latin typeface="+mn-lt"/>
+                                      <a:latin typeface="Cambria Math"/>
                                       <a:ea typeface="+mn-ea"/>
                                       <a:cs typeface="+mn-cs"/>
                                     </a:rPr>
@@ -468,7 +746,7 @@
                                             <a:schemeClr val="tx1"/>
                                           </a:solidFill>
                                           <a:effectLst/>
-                                          <a:latin typeface="+mn-lt"/>
+                                          <a:latin typeface="Cambria Math"/>
                                           <a:ea typeface="+mn-ea"/>
                                           <a:cs typeface="+mn-cs"/>
                                         </a:rPr>
@@ -483,7 +761,7 @@
                                                 <a:schemeClr val="tx1"/>
                                               </a:solidFill>
                                               <a:effectLst/>
-                                              <a:latin typeface="+mn-lt"/>
+                                              <a:latin typeface="Cambria Math"/>
                                               <a:ea typeface="+mn-ea"/>
                                               <a:cs typeface="+mn-cs"/>
                                             </a:rPr>
@@ -496,7 +774,7 @@
                                                 <a:schemeClr val="tx1"/>
                                               </a:solidFill>
                                               <a:effectLst/>
-                                              <a:latin typeface="+mn-lt"/>
+                                              <a:latin typeface="Cambria Math"/>
                                               <a:ea typeface="+mn-ea"/>
                                               <a:cs typeface="+mn-cs"/>
                                             </a:rPr>
@@ -510,7 +788,7 @@
                                                 <a:schemeClr val="tx1"/>
                                               </a:solidFill>
                                               <a:effectLst/>
-                                              <a:latin typeface="+mn-lt"/>
+                                              <a:latin typeface="Cambria Math"/>
                                               <a:ea typeface="+mn-ea"/>
                                               <a:cs typeface="+mn-cs"/>
                                             </a:rPr>
@@ -526,7 +804,7 @@
                                             <a:schemeClr val="tx1"/>
                                           </a:solidFill>
                                           <a:effectLst/>
-                                          <a:latin typeface="+mn-lt"/>
+                                          <a:latin typeface="Cambria Math"/>
                                           <a:ea typeface="+mn-ea"/>
                                           <a:cs typeface="+mn-cs"/>
                                         </a:rPr>
@@ -542,7 +820,7 @@
                                     <a:schemeClr val="tx1"/>
                                   </a:solidFill>
                                   <a:effectLst/>
-                                  <a:latin typeface="+mn-lt"/>
+                                  <a:latin typeface="Cambria Math"/>
                                   <a:ea typeface="+mn-ea"/>
                                   <a:cs typeface="+mn-cs"/>
                                 </a:rPr>
@@ -556,7 +834,7 @@
                                         <a:schemeClr val="tx1"/>
                                       </a:solidFill>
                                       <a:effectLst/>
-                                      <a:latin typeface="+mn-lt"/>
+                                      <a:latin typeface="Cambria Math"/>
                                       <a:ea typeface="+mn-ea"/>
                                       <a:cs typeface="+mn-cs"/>
                                     </a:rPr>
@@ -571,7 +849,7 @@
                                             <a:schemeClr val="tx1"/>
                                           </a:solidFill>
                                           <a:effectLst/>
-                                          <a:latin typeface="+mn-lt"/>
+                                          <a:latin typeface="Cambria Math"/>
                                           <a:ea typeface="+mn-ea"/>
                                           <a:cs typeface="+mn-cs"/>
                                         </a:rPr>
@@ -586,7 +864,7 @@
                                                 <a:schemeClr val="tx1"/>
                                               </a:solidFill>
                                               <a:effectLst/>
-                                              <a:latin typeface="+mn-lt"/>
+                                              <a:latin typeface="Cambria Math"/>
                                               <a:ea typeface="+mn-ea"/>
                                               <a:cs typeface="+mn-cs"/>
                                             </a:rPr>
@@ -599,7 +877,7 @@
                                                 <a:schemeClr val="tx1"/>
                                               </a:solidFill>
                                               <a:effectLst/>
-                                              <a:latin typeface="+mn-lt"/>
+                                              <a:latin typeface="Cambria Math"/>
                                               <a:ea typeface="+mn-ea"/>
                                               <a:cs typeface="+mn-cs"/>
                                             </a:rPr>
@@ -613,7 +891,7 @@
                                                 <a:schemeClr val="tx1"/>
                                               </a:solidFill>
                                               <a:effectLst/>
-                                              <a:latin typeface="+mn-lt"/>
+                                              <a:latin typeface="Cambria Math"/>
                                               <a:ea typeface="+mn-ea"/>
                                               <a:cs typeface="+mn-cs"/>
                                             </a:rPr>
@@ -629,7 +907,7 @@
                                             <a:schemeClr val="tx1"/>
                                           </a:solidFill>
                                           <a:effectLst/>
-                                          <a:latin typeface="+mn-lt"/>
+                                          <a:latin typeface="Cambria Math"/>
                                           <a:ea typeface="+mn-ea"/>
                                           <a:cs typeface="+mn-cs"/>
                                         </a:rPr>
@@ -647,7 +925,7 @@
                                 <a:schemeClr val="tx1"/>
                               </a:solidFill>
                               <a:effectLst/>
-                              <a:latin typeface="+mn-lt"/>
+                              <a:latin typeface="Cambria Math"/>
                               <a:ea typeface="+mn-ea"/>
                               <a:cs typeface="+mn-cs"/>
                             </a:rPr>
@@ -832,7 +1110,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -1079,8 +1357,8 @@
       <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2096343" cy="253339"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -1218,7 +1496,7 @@
                                     <a:schemeClr val="tx1"/>
                                   </a:solidFill>
                                   <a:effectLst/>
-                                  <a:latin typeface="+mn-lt"/>
+                                  <a:latin typeface="Cambria Math"/>
                                   <a:ea typeface="+mn-ea"/>
                                   <a:cs typeface="+mn-cs"/>
                                 </a:rPr>
@@ -1234,7 +1512,7 @@
                                     <a:schemeClr val="tx1"/>
                                   </a:solidFill>
                                   <a:effectLst/>
-                                  <a:latin typeface="+mn-lt"/>
+                                  <a:latin typeface="Cambria Math"/>
                                   <a:ea typeface="+mn-ea"/>
                                   <a:cs typeface="+mn-cs"/>
                                 </a:rPr>
@@ -1251,7 +1529,7 @@
                                         <a:schemeClr val="tx1"/>
                                       </a:solidFill>
                                       <a:effectLst/>
-                                      <a:latin typeface="+mn-lt"/>
+                                      <a:latin typeface="Cambria Math"/>
                                       <a:ea typeface="+mn-ea"/>
                                       <a:cs typeface="+mn-cs"/>
                                     </a:rPr>
@@ -1266,7 +1544,7 @@
                                             <a:schemeClr val="tx1"/>
                                           </a:solidFill>
                                           <a:effectLst/>
-                                          <a:latin typeface="+mn-lt"/>
+                                          <a:latin typeface="Cambria Math"/>
                                           <a:ea typeface="+mn-ea"/>
                                           <a:cs typeface="+mn-cs"/>
                                         </a:rPr>
@@ -1281,7 +1559,7 @@
                                                 <a:schemeClr val="tx1"/>
                                               </a:solidFill>
                                               <a:effectLst/>
-                                              <a:latin typeface="+mn-lt"/>
+                                              <a:latin typeface="Cambria Math"/>
                                               <a:ea typeface="+mn-ea"/>
                                               <a:cs typeface="+mn-cs"/>
                                             </a:rPr>
@@ -1294,7 +1572,7 @@
                                                 <a:schemeClr val="tx1"/>
                                               </a:solidFill>
                                               <a:effectLst/>
-                                              <a:latin typeface="+mn-lt"/>
+                                              <a:latin typeface="Cambria Math"/>
                                               <a:ea typeface="+mn-ea"/>
                                               <a:cs typeface="+mn-cs"/>
                                             </a:rPr>
@@ -1308,7 +1586,7 @@
                                                 <a:schemeClr val="tx1"/>
                                               </a:solidFill>
                                               <a:effectLst/>
-                                              <a:latin typeface="+mn-lt"/>
+                                              <a:latin typeface="Cambria Math"/>
                                               <a:ea typeface="+mn-ea"/>
                                               <a:cs typeface="+mn-cs"/>
                                             </a:rPr>
@@ -1324,7 +1602,7 @@
                                             <a:schemeClr val="tx1"/>
                                           </a:solidFill>
                                           <a:effectLst/>
-                                          <a:latin typeface="+mn-lt"/>
+                                          <a:latin typeface="Cambria Math"/>
                                           <a:ea typeface="+mn-ea"/>
                                           <a:cs typeface="+mn-cs"/>
                                         </a:rPr>
@@ -1340,7 +1618,7 @@
                                     <a:schemeClr val="tx1"/>
                                   </a:solidFill>
                                   <a:effectLst/>
-                                  <a:latin typeface="+mn-lt"/>
+                                  <a:latin typeface="Cambria Math"/>
                                   <a:ea typeface="+mn-ea"/>
                                   <a:cs typeface="+mn-cs"/>
                                 </a:rPr>
@@ -1354,7 +1632,7 @@
                                         <a:schemeClr val="tx1"/>
                                       </a:solidFill>
                                       <a:effectLst/>
-                                      <a:latin typeface="+mn-lt"/>
+                                      <a:latin typeface="Cambria Math"/>
                                       <a:ea typeface="+mn-ea"/>
                                       <a:cs typeface="+mn-cs"/>
                                     </a:rPr>
@@ -1369,7 +1647,7 @@
                                             <a:schemeClr val="tx1"/>
                                           </a:solidFill>
                                           <a:effectLst/>
-                                          <a:latin typeface="+mn-lt"/>
+                                          <a:latin typeface="Cambria Math"/>
                                           <a:ea typeface="+mn-ea"/>
                                           <a:cs typeface="+mn-cs"/>
                                         </a:rPr>
@@ -1384,7 +1662,7 @@
                                                 <a:schemeClr val="tx1"/>
                                               </a:solidFill>
                                               <a:effectLst/>
-                                              <a:latin typeface="+mn-lt"/>
+                                              <a:latin typeface="Cambria Math"/>
                                               <a:ea typeface="+mn-ea"/>
                                               <a:cs typeface="+mn-cs"/>
                                             </a:rPr>
@@ -1397,7 +1675,7 @@
                                                 <a:schemeClr val="tx1"/>
                                               </a:solidFill>
                                               <a:effectLst/>
-                                              <a:latin typeface="+mn-lt"/>
+                                              <a:latin typeface="Cambria Math"/>
                                               <a:ea typeface="+mn-ea"/>
                                               <a:cs typeface="+mn-cs"/>
                                             </a:rPr>
@@ -1411,7 +1689,7 @@
                                                 <a:schemeClr val="tx1"/>
                                               </a:solidFill>
                                               <a:effectLst/>
-                                              <a:latin typeface="+mn-lt"/>
+                                              <a:latin typeface="Cambria Math"/>
                                               <a:ea typeface="+mn-ea"/>
                                               <a:cs typeface="+mn-cs"/>
                                             </a:rPr>
@@ -1427,7 +1705,7 @@
                                             <a:schemeClr val="tx1"/>
                                           </a:solidFill>
                                           <a:effectLst/>
-                                          <a:latin typeface="+mn-lt"/>
+                                          <a:latin typeface="Cambria Math"/>
                                           <a:ea typeface="+mn-ea"/>
                                           <a:cs typeface="+mn-cs"/>
                                         </a:rPr>
@@ -1545,7 +1823,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -1676,22 +1954,27 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>10037</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>105002</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>29087</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>85952</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1704,7 +1987,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8534400" y="1200150"/>
+          <a:off x="6724650" y="2266950"/>
           <a:ext cx="3667637" cy="1629002"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1716,20 +1999,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>19918</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>114543</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>124693</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>9768</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1742,7 +2025,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5991225" y="2914650"/>
+          <a:off x="6705600" y="190500"/>
           <a:ext cx="6220693" cy="1743318"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2085,11 +2368,11 @@
       </c>
       <c r="D5" s="4">
         <f ca="1">2*RAND()*$D$2</f>
-        <v>2.2414128483516027</v>
+        <v>1.0216727255584224</v>
       </c>
       <c r="E5" s="5">
         <f t="shared" ref="E5:E14" ca="1" si="0">(1+C5/360*D5/100)</f>
-        <v>1.0000622614680097</v>
+        <v>1.0000283797979321</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>23</v>
@@ -2104,11 +2387,11 @@
       </c>
       <c r="D6" s="4">
         <f t="shared" ref="D6:D14" ca="1" si="1">2*RAND()*$D$2</f>
-        <v>8.1036664584099007</v>
+        <v>7.708042451149371</v>
       </c>
       <c r="E6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0002251018460668</v>
+        <v>1.0002141122903097</v>
       </c>
       <c r="G6" s="10"/>
     </row>
@@ -2121,11 +2404,11 @@
       </c>
       <c r="D7" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>2.0823053911869338</v>
+        <v>4.5989182640212887</v>
       </c>
       <c r="E7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0000578418164219</v>
+        <v>1.000127747729556</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -2137,11 +2420,11 @@
       </c>
       <c r="D8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>3.0315222844897569</v>
+        <v>6.1178370187801443</v>
       </c>
       <c r="E8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.000084208952347</v>
+        <v>1.0001699399171884</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -2153,11 +2436,11 @@
       </c>
       <c r="D9" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>2.0499830986524561</v>
+        <v>8.2655037768146151</v>
       </c>
       <c r="E9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0001708319248876</v>
+        <v>1.0006887919814011</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -2169,11 +2452,11 @@
       </c>
       <c r="D10" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>5.5505849005523009</v>
+        <v>8.1052803154151203</v>
       </c>
       <c r="E10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0001541829139042</v>
+        <v>1.0002251466754282</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -2185,11 +2468,11 @@
       </c>
       <c r="D11" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>8.2282251577459391</v>
+        <v>3.278831275975429</v>
       </c>
       <c r="E11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0002285618099374</v>
+        <v>1.0000910786465549</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -2201,11 +2484,11 @@
       </c>
       <c r="D12" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>7.2543893541964088</v>
+        <v>9.1531889018235315</v>
       </c>
       <c r="E12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0002015108153943</v>
+        <v>1.0002542552472728</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
@@ -2217,11 +2500,11 @@
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>6.2885970697705815</v>
+        <v>4.9349462982197476</v>
       </c>
       <c r="E13" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.000174683251938</v>
+        <v>1.0001370818416173</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
@@ -2233,11 +2516,11 @@
       </c>
       <c r="D14" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>3.9762344957482321</v>
+        <v>1.6092862315702727</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0003313528746456</v>
+        <v>1.0001341071859642</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="18" x14ac:dyDescent="0.25">
@@ -2258,11 +2541,11 @@
       </c>
       <c r="D17" s="6">
         <f ca="1">SUMPRODUCT(D5:D14,C5:C14)/C17</f>
-        <v>4.3470968748503926</v>
+        <v>5.3245062340069795</v>
       </c>
       <c r="E17" s="6">
         <f ca="1">(PRODUCT(E5:E15)-1)*(360/C17)*100</f>
-        <v>4.3503213099711502</v>
+        <v>5.32908668225694</v>
       </c>
     </row>
     <row r="18" spans="3:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -2305,11 +2588,11 @@
       </c>
       <c r="D23" s="6">
         <f ca="1">100-D17</f>
-        <v>95.652903125149606</v>
+        <v>94.675493765993025</v>
       </c>
       <c r="E23" s="6">
         <f ca="1">100-E17</f>
-        <v>95.64967869002885</v>
+        <v>94.670913317743057</v>
       </c>
     </row>
     <row r="24" spans="3:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -2317,4 +2600,234 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:J18"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="18"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="20"/>
+      <c r="J2" s="21"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="22"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="26"/>
+    </row>
+    <row r="4" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="24"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="28">
+        <v>23</v>
+      </c>
+      <c r="I4" s="25"/>
+      <c r="J4" s="26"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="33"/>
+    </row>
+    <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="1" t="str">
+        <f t="shared" ref="D9:D12" si="0">B9&amp;C9</f>
+        <v>EDH3</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>EDM3</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>EDU3</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>EDZ3</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="18"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="20"/>
+      <c r="J15" s="21"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="22"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="26"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="24"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="28">
+        <v>3</v>
+      </c>
+      <c r="I17" s="25"/>
+      <c r="J17" s="26"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="29"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="33"/>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="B15:D16"/>
+    <mergeCell ref="E15:G16"/>
+    <mergeCell ref="H15:J16"/>
+    <mergeCell ref="B17:D18"/>
+    <mergeCell ref="E17:G18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="B2:D3"/>
+    <mergeCell ref="B4:D5"/>
+    <mergeCell ref="E2:G3"/>
+    <mergeCell ref="E4:G5"/>
+    <mergeCell ref="H2:J3"/>
+    <mergeCell ref="H4:J5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>